<commit_message>
finalized the rough version of the index
</commit_message>
<xml_diff>
--- a/raw_reit_data/centurion/Centurion NAVs and distributions.xlsx
+++ b/raw_reit_data/centurion/Centurion NAVs and distributions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19059\Simple Python Projects\private-reit-simulation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19059\Simple Python Projects\private-reit-simulation\raw_reit_data\centurion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B741858-3D17-4312-AA98-380649E70059}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4F71BF-8FAD-4D67-81F5-0C2B02FFFBEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3015" yWindow="2265" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31080" yWindow="2760" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REIT" sheetId="4" r:id="rId1"/>
@@ -536,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="F130" sqref="F130"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="C141" sqref="C141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2088,17 +2088,93 @@
         <v>6.8330000000000002E-2</v>
       </c>
     </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131" s="8">
+        <v>43922</v>
+      </c>
+      <c r="B131" s="2">
+        <v>18.896000000000001</v>
+      </c>
+      <c r="C131" s="5">
+        <v>6.8330000000000002E-2</v>
+      </c>
+    </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A132" s="7"/>
+      <c r="A132" s="7">
+        <v>43952</v>
+      </c>
+      <c r="B132" s="2">
+        <v>18.896000000000001</v>
+      </c>
+      <c r="C132" s="5">
+        <v>6.8330000000000002E-2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133" s="8">
+        <v>43983</v>
+      </c>
+      <c r="B133" s="2">
+        <v>18.896000000000001</v>
+      </c>
+      <c r="C133" s="5">
+        <v>6.8330000000000002E-2</v>
+      </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A134" s="7"/>
+      <c r="A134" s="7">
+        <v>44013</v>
+      </c>
+      <c r="B134" s="2">
+        <v>18.896000000000001</v>
+      </c>
+      <c r="C134" s="5">
+        <v>6.8330000000000002E-2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135" s="8">
+        <v>44044</v>
+      </c>
+      <c r="B135" s="2">
+        <v>19.242999999999999</v>
+      </c>
+      <c r="C135" s="5">
+        <v>6.8330000000000002E-2</v>
+      </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A136" s="7"/>
+      <c r="A136" s="7">
+        <v>44075</v>
+      </c>
+      <c r="B136" s="2">
+        <v>19.242999999999999</v>
+      </c>
+      <c r="C136" s="5">
+        <v>6.8330000000000002E-2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137" s="8">
+        <v>44105</v>
+      </c>
+      <c r="B137" s="2">
+        <v>19.242999999999999</v>
+      </c>
+      <c r="C137" s="5">
+        <v>6.8330000000000002E-2</v>
+      </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A138" s="7"/>
+      <c r="A138" s="7">
+        <v>44136</v>
+      </c>
+      <c r="B138" s="2">
+        <v>19.34</v>
+      </c>
+      <c r="C138" s="5">
+        <v>6.8330000000000002E-2</v>
+      </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" s="7"/>

</xml_diff>